<commit_message>
commit ticket configure stage 1
</commit_message>
<xml_diff>
--- a/AMSWebserver/src/test/resources/TestData.xlsx
+++ b/AMSWebserver/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/premsanil/git/AMS/AMSWebserver/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF5A859-9EB4-3344-9B76-3613649BA128}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78312E23-5AA8-1648-8C66-B2F86D2B37B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16060" activeTab="4" xr2:uid="{05DF50FA-CBB6-C140-9382-A694CFC3DB6B}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16060" activeTab="8" xr2:uid="{05DF50FA-CBB6-C140-9382-A694CFC3DB6B}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
     <sheet name="FormParameterData" sheetId="5" r:id="rId5"/>
     <sheet name="FormTypedata" sheetId="6" r:id="rId6"/>
+    <sheet name="Department" sheetId="7" r:id="rId7"/>
+    <sheet name="SubDepartment" sheetId="8" r:id="rId8"/>
+    <sheet name="Manufacture" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="175">
   <si>
     <t>UD</t>
   </si>
@@ -427,9 +430,6 @@
     <t>FALSE</t>
   </si>
   <si>
-    <t>Raf_label01</t>
-  </si>
-  <si>
     <t>Automation</t>
   </si>
   <si>
@@ -442,9 +442,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Auto_1296</t>
-  </si>
-  <si>
     <t>Type Id</t>
   </si>
   <si>
@@ -505,28 +502,67 @@
     <t>rafeek</t>
   </si>
   <si>
-    <t>Auto-015</t>
-  </si>
-  <si>
-    <t>Automation25</t>
-  </si>
-  <si>
     <t>Number</t>
   </si>
   <si>
     <t>100</t>
   </si>
   <si>
-    <t>Auto-199</t>
-  </si>
-  <si>
-    <t>Automation287</t>
-  </si>
-  <si>
-    <t>Auto_76565</t>
-  </si>
-  <si>
-    <t>Raf_label7654</t>
+    <t>Auto_561</t>
+  </si>
+  <si>
+    <t>Auto_562</t>
+  </si>
+  <si>
+    <t>Raf_label561</t>
+  </si>
+  <si>
+    <t>Raf_labeL562</t>
+  </si>
+  <si>
+    <t>Auto-561</t>
+  </si>
+  <si>
+    <t>Auto-562</t>
+  </si>
+  <si>
+    <t>Automation561</t>
+  </si>
+  <si>
+    <t>Automation562</t>
+  </si>
+  <si>
+    <t>Department Id</t>
+  </si>
+  <si>
+    <t>Metadata</t>
+  </si>
+  <si>
+    <t>Auto-124</t>
+  </si>
+  <si>
+    <t>Auto-125</t>
+  </si>
+  <si>
+    <t>sub Department Id</t>
+  </si>
+  <si>
+    <t>Manufacture Id</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Auto-SD130</t>
+  </si>
+  <si>
+    <t>Auto-SD131</t>
+  </si>
+  <si>
+    <t>Auto-MID132</t>
+  </si>
+  <si>
+    <t>Auto-MID133</t>
   </si>
 </sst>
 </file>
@@ -1791,7 +1827,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C28"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2113,8 +2149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76886557-E3C0-7543-9BD4-05C08338B35B}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2147,21 +2183,21 @@
         <v>126</v>
       </c>
       <c r="G1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" t="s">
         <v>132</v>
-      </c>
-      <c r="H1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
       <c r="B2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" t="s">
         <v>130</v>
-      </c>
-      <c r="C2" t="s">
-        <v>131</v>
       </c>
       <c r="D2" t="s">
         <v>128</v>
@@ -2173,36 +2209,36 @@
         <v>127</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>129</v>
       </c>
       <c r="F3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>49</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2216,129 +2252,129 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" t="s">
         <v>136</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>137</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>138</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>139</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>140</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>141</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>142</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>143</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>144</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>145</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>146</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>147</v>
-      </c>
-      <c r="M1" t="s">
-        <v>148</v>
-      </c>
-      <c r="N1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H2" t="s">
+        <v>148</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="J2" t="s">
         <v>150</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="K2" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="N2" t="s">
         <v>151</v>
-      </c>
-      <c r="J2" t="s">
-        <v>152</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="N2" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B3" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>129</v>
       </c>
       <c r="J3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>129</v>
@@ -2350,7 +2386,173 @@
         <v>129</v>
       </c>
       <c r="N3" t="s">
-        <v>153</v>
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CE29F11-D419-E34D-8103-7F124FCAB900}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E414F2-882A-9B4E-99BF-1CD7EF37A74D}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D419BF-B4A0-674F-B567-3CEE0078DF3B}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Asset addition and validation added
</commit_message>
<xml_diff>
--- a/AMSWebserver/src/test/resources/TestData.xlsx
+++ b/AMSWebserver/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/premsanil/git/AMS/AMSWebserver/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD0E54E-F186-5941-905A-38FC2EA64972}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBD7D39-1488-D844-BE1C-66528B48EC47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" firstSheet="2" activeTab="14" xr2:uid="{05DF50FA-CBB6-C140-9382-A694CFC3DB6B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" firstSheet="3" activeTab="15" xr2:uid="{05DF50FA-CBB6-C140-9382-A694CFC3DB6B}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData1" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <sheet name="Location" sheetId="13" r:id="rId13"/>
     <sheet name="AssetMap" sheetId="14" r:id="rId14"/>
     <sheet name="User" sheetId="15" r:id="rId15"/>
+    <sheet name="Asset" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="289">
   <si>
     <t>UD</t>
   </si>
@@ -556,9 +557,6 @@
     <t>Manufacture Id</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
     <t>Auto-SD130</t>
   </si>
   <si>
@@ -776,6 +774,144 @@
   </si>
   <si>
     <t>user4untangled@gmail.com</t>
+  </si>
+  <si>
+    <t>Auto-UID003</t>
+  </si>
+  <si>
+    <t>Auto_tester3</t>
+  </si>
+  <si>
+    <t>12.35</t>
+  </si>
+  <si>
+    <t>34.569</t>
+  </si>
+  <si>
+    <t>05:03:02</t>
+  </si>
+  <si>
+    <t>Auto-LID010</t>
+  </si>
+  <si>
+    <t>Auto-LID11</t>
+  </si>
+  <si>
+    <t>Auto-LID12</t>
+  </si>
+  <si>
+    <t>12.36</t>
+  </si>
+  <si>
+    <t>12.37123</t>
+  </si>
+  <si>
+    <t>34.570</t>
+  </si>
+  <si>
+    <t>34.571</t>
+  </si>
+  <si>
+    <t>05:03:03</t>
+  </si>
+  <si>
+    <t>05:03:04</t>
+  </si>
+  <si>
+    <t>Technician</t>
+  </si>
+  <si>
+    <t>Asset ID</t>
+  </si>
+  <si>
+    <t>Tag ID</t>
+  </si>
+  <si>
+    <t>Asset type id</t>
+  </si>
+  <si>
+    <t>department ID</t>
+  </si>
+  <si>
+    <t>Sub department ID</t>
+  </si>
+  <si>
+    <t>AMC Expiry</t>
+  </si>
+  <si>
+    <t>bought price</t>
+  </si>
+  <si>
+    <t>current price</t>
+  </si>
+  <si>
+    <t>location ID</t>
+  </si>
+  <si>
+    <t>Vendor Company ID</t>
+  </si>
+  <si>
+    <t>Asset Type</t>
+  </si>
+  <si>
+    <t>Manufacturer ID</t>
+  </si>
+  <si>
+    <t>Model ID</t>
+  </si>
+  <si>
+    <t>Meta Data</t>
+  </si>
+  <si>
+    <t>Installation Date</t>
+  </si>
+  <si>
+    <t>Latest service Date</t>
+  </si>
+  <si>
+    <t>Next service Date</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>Technician ID</t>
+  </si>
+  <si>
+    <t>User Notify ID</t>
+  </si>
+  <si>
+    <t>Auto-Asset</t>
+  </si>
+  <si>
+    <t>Auto-TID01</t>
+  </si>
+  <si>
+    <t>01/10/2023</t>
+  </si>
+  <si>
+    <t>25000</t>
+  </si>
+  <si>
+    <t>20000</t>
+  </si>
+  <si>
+    <t>VC01</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Auto-MID140</t>
+  </si>
+  <si>
+    <t>1/17/2023</t>
+  </si>
+  <si>
+    <t>3/28/2023</t>
+  </si>
+  <si>
+    <t>1/9/2023</t>
   </si>
 </sst>
 </file>
@@ -838,13 +974,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1661,7 +1798,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -1672,7 +1809,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B2" t="s">
         <v>130</v>
@@ -1683,7 +1820,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B3" t="s">
         <v>130</v>
@@ -1710,7 +1847,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -1721,7 +1858,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B2" t="s">
         <v>130</v>
@@ -1732,7 +1869,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B3" t="s">
         <v>130</v>
@@ -1764,7 +1901,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -1775,7 +1912,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B2" t="s">
         <v>130</v>
@@ -1786,7 +1923,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B3" t="s">
         <v>130</v>
@@ -1803,10 +1940,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED28C11-1986-AA4D-ACB3-1BED2DC8CC0B}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1821,71 +1958,140 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" t="s">
         <v>184</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>185</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>186</v>
-      </c>
-      <c r="D1" t="s">
-        <v>187</v>
       </c>
       <c r="E1" t="s">
         <v>165</v>
       </c>
       <c r="F1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G1" t="s">
         <v>188</v>
-      </c>
-      <c r="G1" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" t="s">
         <v>193</v>
       </c>
-      <c r="E2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F2" t="s">
-        <v>194</v>
-      </c>
       <c r="G2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>198</v>
+        <v>248</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" t="s">
+        <v>193</v>
+      </c>
+      <c r="G3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>197</v>
       </c>
-      <c r="E3" t="s">
-        <v>130</v>
-      </c>
-      <c r="F3" t="s">
-        <v>194</v>
-      </c>
-      <c r="G3" t="s">
-        <v>183</v>
+      <c r="B4" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F4" t="s">
+        <v>193</v>
+      </c>
+      <c r="G4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="E5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5" t="s">
+        <v>193</v>
+      </c>
+      <c r="G5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6" t="s">
+        <v>193</v>
+      </c>
+      <c r="G6" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -1911,13 +2117,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D1" t="s">
         <v>165</v>
@@ -1925,13 +2131,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B2" t="s">
         <v>130</v>
       </c>
       <c r="C2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D2" t="s">
         <v>130</v>
@@ -1939,13 +2145,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B3" t="s">
         <v>130</v>
       </c>
       <c r="C3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D3" t="s">
         <v>130</v>
@@ -1959,10 +2165,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{993EA0DD-74C0-674B-B9F1-BC88BECF4A75}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1972,170 +2178,226 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" t="s">
         <v>205</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>206</v>
-      </c>
-      <c r="C1" t="s">
-        <v>207</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
       </c>
       <c r="E1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F1" t="s">
         <v>208</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>209</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>210</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>211</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>212</v>
-      </c>
-      <c r="J1" t="s">
-        <v>213</v>
       </c>
       <c r="K1" t="s">
         <v>165</v>
       </c>
       <c r="L1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M1" t="s">
         <v>214</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>215</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>216</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>217</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>218</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>219</v>
-      </c>
-      <c r="R1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" t="s">
         <v>221</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="F2" t="s">
         <v>222</v>
       </c>
-      <c r="C2" t="s">
-        <v>222</v>
-      </c>
-      <c r="D2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="F2" t="s">
-        <v>223</v>
-      </c>
       <c r="G2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="J2" t="s">
         <v>225</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
+        <v>130</v>
+      </c>
+      <c r="L2" t="s">
         <v>226</v>
       </c>
-      <c r="K2" t="s">
-        <v>130</v>
-      </c>
-      <c r="L2" t="s">
-        <v>227</v>
-      </c>
       <c r="M2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="N2" t="s">
+        <v>230</v>
+      </c>
+      <c r="O2" t="s">
         <v>231</v>
       </c>
-      <c r="O2" t="s">
-        <v>232</v>
-      </c>
       <c r="P2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="R2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="F3" t="s">
+        <v>223</v>
+      </c>
+      <c r="G3" t="s">
+        <v>240</v>
+      </c>
+      <c r="H3" t="s">
+        <v>240</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="J3" t="s">
         <v>239</v>
       </c>
-      <c r="B3" t="s">
-        <v>241</v>
-      </c>
-      <c r="C3" t="s">
-        <v>241</v>
-      </c>
-      <c r="D3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="F3" t="s">
-        <v>224</v>
-      </c>
-      <c r="G3" t="s">
-        <v>241</v>
-      </c>
-      <c r="H3" t="s">
-        <v>241</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="J3" t="s">
-        <v>240</v>
-      </c>
       <c r="K3" t="s">
         <v>130</v>
       </c>
       <c r="L3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N3" t="s">
         <v>167</v>
       </c>
       <c r="O3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P3" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q3" t="s">
         <v>235</v>
       </c>
-      <c r="Q3" t="s">
-        <v>236</v>
-      </c>
       <c r="R3" t="s">
-        <v>238</v>
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C4" t="s">
+        <v>240</v>
+      </c>
+      <c r="D4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="F4" t="s">
+        <v>223</v>
+      </c>
+      <c r="G4" t="s">
+        <v>240</v>
+      </c>
+      <c r="H4" t="s">
+        <v>240</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="J4" t="s">
+        <v>239</v>
+      </c>
+      <c r="K4" t="s">
+        <v>130</v>
+      </c>
+      <c r="L4" t="s">
+        <v>244</v>
+      </c>
+      <c r="M4" t="s">
+        <v>229</v>
+      </c>
+      <c r="N4" t="s">
+        <v>167</v>
+      </c>
+      <c r="O4" t="s">
+        <v>232</v>
+      </c>
+      <c r="P4" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>235</v>
+      </c>
+      <c r="R4" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -2143,7 +2405,147 @@
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{BB4670C8-CDFD-B445-B287-73C12D212D27}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{DB1B16BB-5677-D34A-AD08-4509D79A03AE}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{318831B5-8275-5C44-B5DA-DCE23E276C86}"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0588CAB-E2D0-C44A-A810-90E391CD495F}">
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E1" t="s">
+        <v>262</v>
+      </c>
+      <c r="F1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" t="s">
+        <v>264</v>
+      </c>
+      <c r="H1" t="s">
+        <v>265</v>
+      </c>
+      <c r="I1" t="s">
+        <v>266</v>
+      </c>
+      <c r="J1" t="s">
+        <v>267</v>
+      </c>
+      <c r="K1" t="s">
+        <v>268</v>
+      </c>
+      <c r="L1" t="s">
+        <v>269</v>
+      </c>
+      <c r="M1" t="s">
+        <v>270</v>
+      </c>
+      <c r="N1" t="s">
+        <v>271</v>
+      </c>
+      <c r="O1" t="s">
+        <v>272</v>
+      </c>
+      <c r="P1" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>274</v>
+      </c>
+      <c r="R1" t="s">
+        <v>275</v>
+      </c>
+      <c r="S1" t="s">
+        <v>276</v>
+      </c>
+      <c r="T1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I2" t="s">
+        <v>249</v>
+      </c>
+      <c r="J2" t="s">
+        <v>283</v>
+      </c>
+      <c r="K2" t="s">
+        <v>284</v>
+      </c>
+      <c r="L2" t="s">
+        <v>285</v>
+      </c>
+      <c r="M2" t="s">
+        <v>175</v>
+      </c>
+      <c r="N2" t="s">
+        <v>130</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="R2" t="s">
+        <v>130</v>
+      </c>
+      <c r="S2" t="s">
+        <v>222</v>
+      </c>
+      <c r="T2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3204,7 +3606,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B2" t="s">
         <v>130</v>
@@ -3215,7 +3617,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B3" t="s">
         <v>130</v>
@@ -3232,10 +3634,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D419BF-B4A0-674F-B567-3CEE0078DF3B}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C3"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3258,7 +3660,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" t="s">
         <v>130</v>
@@ -3269,18 +3671,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B3" t="s">
         <v>130</v>
       </c>
       <c r="C3" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
-        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AMS WEBSERVER PING TESTING
</commit_message>
<xml_diff>
--- a/AMSWebserver/src/test/resources/TestData.xlsx
+++ b/AMSWebserver/src/test/resources/TestData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/premsanil/git/AMS/AMSWebserver/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7728E5A7-DD58-BD4A-8799-66B1B41C460E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B770277-9EC3-C24E-8B63-74B5DA8CD432}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" firstSheet="6" activeTab="18" xr2:uid="{05DF50FA-CBB6-C140-9382-A694CFC3DB6B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" firstSheet="7" activeTab="15" xr2:uid="{05DF50FA-CBB6-C140-9382-A694CFC3DB6B}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData1" sheetId="1" r:id="rId1"/>
@@ -29,19 +29,21 @@
     <sheet name="Location" sheetId="13" r:id="rId14"/>
     <sheet name="AssetMap" sheetId="14" r:id="rId15"/>
     <sheet name="User" sheetId="15" r:id="rId16"/>
-    <sheet name="Asset" sheetId="16" r:id="rId17"/>
-    <sheet name="Role" sheetId="19" r:id="rId18"/>
-    <sheet name="MQTT" sheetId="20" r:id="rId19"/>
-    <sheet name="VendorCompany" sheetId="18" r:id="rId20"/>
+    <sheet name="Sheet2" sheetId="21" r:id="rId17"/>
+    <sheet name="Asset" sheetId="16" r:id="rId18"/>
+    <sheet name="Role" sheetId="19" r:id="rId19"/>
+    <sheet name="MQTT" sheetId="20" r:id="rId20"/>
+    <sheet name="VendorCompany" sheetId="18" r:id="rId21"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -49,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="373">
   <si>
     <t>UD</t>
   </si>
@@ -579,21 +581,6 @@
     <t>Visible</t>
   </si>
   <si>
-    <t>Auto_tester1</t>
-  </si>
-  <si>
-    <t>Auto_001</t>
-  </si>
-  <si>
-    <t>Auto-SD123</t>
-  </si>
-  <si>
-    <t>Role1</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
     <t>Asset type id</t>
   </si>
   <si>
@@ -669,9 +656,6 @@
     <t>1/9/2023</t>
   </si>
   <si>
-    <t>UID1234</t>
-  </si>
-  <si>
     <t>Comment Header</t>
   </si>
   <si>
@@ -783,21 +767,9 @@
     <t>123456789</t>
   </si>
   <si>
-    <t>Auto_tester2</t>
-  </si>
-  <si>
     <t>Disable</t>
   </si>
   <si>
-    <t>QA</t>
-  </si>
-  <si>
-    <t>def@gmail.com</t>
-  </si>
-  <si>
-    <t>xyz@gmail.com</t>
-  </si>
-  <si>
     <t>Mqtt ID</t>
   </si>
   <si>
@@ -834,18 +806,6 @@
     <t>Ashish</t>
   </si>
   <si>
-    <t>Mqtt_01</t>
-  </si>
-  <si>
-    <t>Software</t>
-  </si>
-  <si>
-    <t>Hardware</t>
-  </si>
-  <si>
-    <t>Development</t>
-  </si>
-  <si>
     <t>Machines part</t>
   </si>
   <si>
@@ -915,9 +875,6 @@
     <t>1699939990374</t>
   </si>
   <si>
-    <t>1699939997643</t>
-  </si>
-  <si>
     <t>1699939999721</t>
   </si>
   <si>
@@ -954,9 +911,6 @@
     <t>Time Multiplier</t>
   </si>
   <si>
-    <t>1700139425755</t>
-  </si>
-  <si>
     <t xml:space="preserve">Host </t>
   </si>
   <si>
@@ -993,18 +947,236 @@
     <t>A1brk@T3s!</t>
   </si>
   <si>
-    <t>1700144042948</t>
-  </si>
-  <si>
     <t>1700144244340</t>
+  </si>
+  <si>
+    <t>1700197121464</t>
+  </si>
+  <si>
+    <t>user id</t>
+  </si>
+  <si>
+    <t>Nithin H K</t>
+  </si>
+  <si>
+    <t>Somashekar C</t>
+  </si>
+  <si>
+    <t>Nandakumar K N</t>
+  </si>
+  <si>
+    <t>Kiran Kumar</t>
+  </si>
+  <si>
+    <t>Rajendra R</t>
+  </si>
+  <si>
+    <t>Madhu C</t>
+  </si>
+  <si>
+    <t>Venkateshappa M</t>
+  </si>
+  <si>
+    <t>Jaishal</t>
+  </si>
+  <si>
+    <t>Nagaraj N S</t>
+  </si>
+  <si>
+    <t>Vasanth Kumar P</t>
+  </si>
+  <si>
+    <t>Trilokchandra M</t>
+  </si>
+  <si>
+    <t>Manjunatha K N</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>nithin.h@seg-automotive.com</t>
+  </si>
+  <si>
+    <t>somashekar.c@seg-automotive.com</t>
+  </si>
+  <si>
+    <t>nandakumar.kn@seg-automotive.com</t>
+  </si>
+  <si>
+    <t>external.kiran.kumar@seg-automotive.com</t>
+  </si>
+  <si>
+    <t>rajendra.r@seg-automotive.com</t>
+  </si>
+  <si>
+    <t>madhu.c@seg-automotive.com</t>
+  </si>
+  <si>
+    <t>venkateshappa.m@seg-automotive.com</t>
+  </si>
+  <si>
+    <t>external.jaishal.rai@seg-automotive.com</t>
+  </si>
+  <si>
+    <t>nagaraj.salimani@seg-automotive.com</t>
+  </si>
+  <si>
+    <t>vasanth.p@seg-automotive.com</t>
+  </si>
+  <si>
+    <t>trilokchandra.m@seg-automotive.com</t>
+  </si>
+  <si>
+    <t>kn.manjunatha@seg-automotive.com</t>
+  </si>
+  <si>
+    <t>+918197734191</t>
+  </si>
+  <si>
+    <t>+919916917141</t>
+  </si>
+  <si>
+    <t>+919901454947</t>
+  </si>
+  <si>
+    <t>+918892341149</t>
+  </si>
+  <si>
+    <t>+919731499665</t>
+  </si>
+  <si>
+    <t>+916364856784</t>
+  </si>
+  <si>
+    <t>+919901454933</t>
+  </si>
+  <si>
+    <t>+918971185154</t>
+  </si>
+  <si>
+    <t>+919740854645</t>
+  </si>
+  <si>
+    <t>+919986856766</t>
+  </si>
+  <si>
+    <t>+919902016735</t>
+  </si>
+  <si>
+    <t>+919972755668</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>Mantenanace</t>
+  </si>
+  <si>
+    <t>Sub-Assembly</t>
+  </si>
+  <si>
+    <t>Electricla</t>
+  </si>
+  <si>
+    <t>Mechanical</t>
+  </si>
+  <si>
+    <t>FLM</t>
+  </si>
+  <si>
+    <t>Janardhan M</t>
+  </si>
+  <si>
+    <t>Suresh Babu S</t>
+  </si>
+  <si>
+    <t>Samiulla Syed</t>
+  </si>
+  <si>
+    <t>janardhan.m@seg-automotive.com</t>
+  </si>
+  <si>
+    <t>sureshbabu.s@seg-automotive.com</t>
+  </si>
+  <si>
+    <t>syed.samiullah@seg-automotive.com</t>
+  </si>
+  <si>
+    <t>30678703</t>
+  </si>
+  <si>
+    <t>30681496</t>
+  </si>
+  <si>
+    <t>30674440</t>
+  </si>
+  <si>
+    <t>Sunil Kumar S A</t>
+  </si>
+  <si>
+    <t>Kandan M</t>
+  </si>
+  <si>
+    <t>sunil.kumarsa@seg-automotive.com</t>
+  </si>
+  <si>
+    <t>kandan.m@seg-automotive.com</t>
+  </si>
+  <si>
+    <t>+919880001743</t>
+  </si>
+  <si>
+    <t>+918056244799</t>
+  </si>
+  <si>
+    <t>+919880780423</t>
+  </si>
+  <si>
+    <t>+919901454944</t>
+  </si>
+  <si>
+    <t>+919740983880</t>
+  </si>
+  <si>
+    <t>30673833</t>
+  </si>
+  <si>
+    <t>30681138</t>
+  </si>
+  <si>
+    <t>30672647</t>
+  </si>
+  <si>
+    <t>SEG_AUTOMOTIVE</t>
+  </si>
+  <si>
+    <t>SEG AUTOMOTIVE</t>
+  </si>
+  <si>
+    <t>Assembly</t>
+  </si>
+  <si>
+    <t>Seg.@123</t>
+  </si>
+  <si>
+    <t>Electrical</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1038,6 +1210,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1047,10 +1253,36 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -1060,7 +1292,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -1068,6 +1300,47 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1391,10 +1664,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="16.83203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="3" max="4" width="16.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -1877,8 +2150,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="20.33203125" collapsed="true"/>
+    <col min="1" max="1" width="21" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -1891,7 +2164,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="B2" t="s">
         <v>128</v>
@@ -1899,7 +2172,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="B3" t="s">
         <v>128</v>
@@ -1921,8 +2194,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="1" max="1" width="17" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -1935,7 +2208,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="B2" t="s">
         <v>128</v>
@@ -1943,7 +2216,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="B3" t="s">
         <v>128</v>
@@ -1975,7 +2248,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B2" t="s">
         <v>128</v>
@@ -1983,7 +2256,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="B3" t="s">
         <v>128</v>
@@ -2005,8 +2278,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.1640625" collapsed="true"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -2019,7 +2292,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="B2" t="s">
         <v>128</v>
@@ -2027,7 +2300,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="B3" t="s">
         <v>128</v>
@@ -2049,11 +2322,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.1640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="14.83203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.5" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.83203125" collapsed="true"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.5" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -2093,7 +2366,7 @@
         <v>153</v>
       </c>
       <c r="F2" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2113,7 +2386,7 @@
         <v>153</v>
       </c>
       <c r="F3" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -2132,8 +2405,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.83203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.1640625" collapsed="true"/>
+    <col min="1" max="1" width="11.83203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -2152,7 +2425,7 @@
         <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="C2" t="s">
         <v>128</v>
@@ -2166,223 +2439,2519 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{993EA0DD-74C0-674B-B9F1-BC88BECF4A75}">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:V18"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="8" customWidth="true" width="24.5" collapsed="true"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
+    <col min="9" max="9" width="24.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B1" t="s">
         <v>158</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>159</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>160</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>161</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>162</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>163</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>164</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>165</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>144</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>166</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>167</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>168</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>169</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>170</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>171</v>
       </c>
-      <c r="Q1" t="s">
-        <v>239</v>
-      </c>
       <c r="R1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="S1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="T1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="U1" t="s">
+        <v>236</v>
+      </c>
+      <c r="V1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>245</v>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" s="10">
+        <v>30672647</v>
       </c>
       <c r="B2" t="s">
-        <v>173</v>
+        <v>238</v>
       </c>
       <c r="C2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="E2" t="s">
-        <v>206</v>
-      </c>
-      <c r="F2" t="s">
-        <v>173</v>
+        <v>238</v>
+      </c>
+      <c r="D2" t="s">
+        <v>367</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>363</v>
       </c>
       <c r="G2" t="s">
         <v>173</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="H2" t="s">
+        <v>238</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="J2" t="s">
         <v>175</v>
       </c>
-      <c r="J2" t="s">
-        <v>128</v>
-      </c>
       <c r="K2" t="s">
-        <v>176</v>
-      </c>
-      <c r="L2" t="s">
-        <v>177</v>
-      </c>
-      <c r="M2" t="s">
-        <v>282</v>
-      </c>
-      <c r="N2" t="s">
-        <v>178</v>
-      </c>
-      <c r="O2" t="s">
+        <v>313</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="M2" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N2" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="O2" s="20" t="s">
+        <v>370</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S2" t="s">
+        <v>238</v>
+      </c>
+      <c r="T2" t="s">
+        <v>173</v>
+      </c>
+      <c r="U2" t="s">
+        <v>238</v>
+      </c>
+      <c r="V2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" s="10">
+        <v>30681138</v>
+      </c>
+      <c r="B3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C3" t="s">
+        <v>238</v>
+      </c>
+      <c r="D3" t="s">
+        <v>367</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="G3" t="s">
+        <v>173</v>
+      </c>
+      <c r="H3" t="s">
+        <v>238</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="J3" t="s">
+        <v>175</v>
+      </c>
+      <c r="K3" t="s">
+        <v>313</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>354</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N3" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="O3" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="P3" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q3" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S3" t="s">
+        <v>238</v>
+      </c>
+      <c r="T3" t="s">
+        <v>173</v>
+      </c>
+      <c r="U3" t="s">
+        <v>238</v>
+      </c>
+      <c r="V3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" s="10">
+        <v>30674440</v>
+      </c>
+      <c r="B4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D4" t="s">
+        <v>367</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="F4" s="17">
+        <v>30672647</v>
+      </c>
+      <c r="G4" t="s">
+        <v>173</v>
+      </c>
+      <c r="H4" t="s">
+        <v>238</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>360</v>
+      </c>
+      <c r="J4" t="s">
+        <v>175</v>
+      </c>
+      <c r="K4" t="s">
+        <v>313</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="M4" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N4" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="O4" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="P4" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q4" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S4" t="s">
+        <v>238</v>
+      </c>
+      <c r="T4" t="s">
+        <v>173</v>
+      </c>
+      <c r="U4" t="s">
+        <v>238</v>
+      </c>
+      <c r="V4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5" s="10">
+        <v>30681496</v>
+      </c>
+      <c r="B5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D5" t="s">
+        <v>367</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="G5" t="s">
+        <v>173</v>
+      </c>
+      <c r="H5" t="s">
+        <v>238</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>362</v>
+      </c>
+      <c r="J5" t="s">
+        <v>175</v>
+      </c>
+      <c r="K5" t="s">
+        <v>313</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="M5" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N5" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="O5" s="20" t="s">
+        <v>370</v>
+      </c>
+      <c r="P5" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q5" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S5" t="s">
+        <v>238</v>
+      </c>
+      <c r="T5" t="s">
+        <v>173</v>
+      </c>
+      <c r="U5" t="s">
+        <v>238</v>
+      </c>
+      <c r="V5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="10">
+        <v>30678703</v>
+      </c>
+      <c r="B6" t="s">
+        <v>238</v>
+      </c>
+      <c r="C6" t="s">
+        <v>238</v>
+      </c>
+      <c r="D6" t="s">
+        <v>367</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>364</v>
+      </c>
+      <c r="G6" t="s">
+        <v>173</v>
+      </c>
+      <c r="H6" t="s">
+        <v>238</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="J6" t="s">
+        <v>175</v>
+      </c>
+      <c r="K6" t="s">
+        <v>313</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="M6" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N6" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="O6" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="P6" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q6" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S6" t="s">
+        <v>238</v>
+      </c>
+      <c r="T6" t="s">
+        <v>173</v>
+      </c>
+      <c r="U6" t="s">
+        <v>238</v>
+      </c>
+      <c r="V6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>32087330</v>
+      </c>
+      <c r="B7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C7" t="s">
+        <v>238</v>
+      </c>
+      <c r="D7" t="s">
+        <v>367</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="G7" t="s">
+        <v>173</v>
+      </c>
+      <c r="H7" t="s">
+        <v>238</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="J7" t="s">
+        <v>175</v>
+      </c>
+      <c r="K7" t="s">
+        <v>313</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="M7" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N7" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="O7" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="P7" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q7" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S7" t="s">
+        <v>238</v>
+      </c>
+      <c r="T7" t="s">
+        <v>173</v>
+      </c>
+      <c r="U7" t="s">
+        <v>238</v>
+      </c>
+      <c r="V7" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>31175834</v>
+      </c>
+      <c r="B8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C8" t="s">
+        <v>238</v>
+      </c>
+      <c r="D8" t="s">
+        <v>367</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="G8" t="s">
+        <v>173</v>
+      </c>
+      <c r="H8" t="s">
+        <v>238</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="J8" t="s">
+        <v>175</v>
+      </c>
+      <c r="K8" t="s">
+        <v>313</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N8" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="O8" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="P8" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q8" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S8" t="s">
+        <v>238</v>
+      </c>
+      <c r="T8" t="s">
+        <v>173</v>
+      </c>
+      <c r="U8" t="s">
+        <v>238</v>
+      </c>
+      <c r="V8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>33625544</v>
+      </c>
+      <c r="B9" t="s">
+        <v>238</v>
+      </c>
+      <c r="C9" t="s">
+        <v>238</v>
+      </c>
+      <c r="D9" t="s">
+        <v>367</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="G9" t="s">
+        <v>173</v>
+      </c>
+      <c r="H9" t="s">
+        <v>238</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="J9" t="s">
+        <v>175</v>
+      </c>
+      <c r="K9" t="s">
+        <v>313</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="M9" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N9" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="O9" s="20" t="s">
+        <v>370</v>
+      </c>
+      <c r="P9" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q9" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S9" t="s">
+        <v>238</v>
+      </c>
+      <c r="T9" t="s">
+        <v>173</v>
+      </c>
+      <c r="U9" t="s">
+        <v>238</v>
+      </c>
+      <c r="V9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
+        <v>30682333</v>
+      </c>
+      <c r="B10" t="s">
+        <v>238</v>
+      </c>
+      <c r="C10" t="s">
+        <v>238</v>
+      </c>
+      <c r="D10" t="s">
+        <v>367</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="G10" t="s">
+        <v>173</v>
+      </c>
+      <c r="H10" t="s">
+        <v>238</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="J10" t="s">
+        <v>175</v>
+      </c>
+      <c r="K10" t="s">
+        <v>313</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="M10" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N10" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="O10" s="20" t="s">
+        <v>370</v>
+      </c>
+      <c r="P10" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q10" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S10" t="s">
+        <v>238</v>
+      </c>
+      <c r="T10" t="s">
+        <v>173</v>
+      </c>
+      <c r="U10" t="s">
+        <v>238</v>
+      </c>
+      <c r="V10" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A11" s="8">
+        <v>33625753</v>
+      </c>
+      <c r="B11" t="s">
+        <v>238</v>
+      </c>
+      <c r="C11" t="s">
+        <v>238</v>
+      </c>
+      <c r="D11" t="s">
+        <v>367</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="G11" t="s">
+        <v>173</v>
+      </c>
+      <c r="H11" t="s">
+        <v>238</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="J11" t="s">
+        <v>175</v>
+      </c>
+      <c r="K11" t="s">
+        <v>313</v>
+      </c>
+      <c r="L11" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="P2" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="R2" t="s">
-        <v>173</v>
-      </c>
-      <c r="S2" t="s">
-        <v>245</v>
-      </c>
-      <c r="T2" t="s">
-        <v>173</v>
-      </c>
-      <c r="U2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>173</v>
-      </c>
-      <c r="B3" t="s">
-        <v>245</v>
-      </c>
-      <c r="C3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="E3" t="s">
-        <v>206</v>
-      </c>
-      <c r="F3" t="s">
-        <v>173</v>
-      </c>
-      <c r="G3" t="s">
-        <v>173</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="M11" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N11" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="O11" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="P11" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q11" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S11" t="s">
+        <v>238</v>
+      </c>
+      <c r="T11" t="s">
+        <v>173</v>
+      </c>
+      <c r="U11" t="s">
+        <v>238</v>
+      </c>
+      <c r="V11" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A12" s="8">
+        <v>31621727</v>
+      </c>
+      <c r="B12" t="s">
+        <v>238</v>
+      </c>
+      <c r="C12" t="s">
+        <v>238</v>
+      </c>
+      <c r="D12" t="s">
+        <v>367</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="G12" t="s">
+        <v>173</v>
+      </c>
+      <c r="H12" t="s">
+        <v>238</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="J12" t="s">
         <v>175</v>
       </c>
-      <c r="J3" t="s">
-        <v>128</v>
-      </c>
-      <c r="K3" t="s">
-        <v>244</v>
-      </c>
-      <c r="L3" t="s">
-        <v>177</v>
-      </c>
-      <c r="M3" t="s">
-        <v>283</v>
-      </c>
-      <c r="N3" t="s">
-        <v>178</v>
-      </c>
-      <c r="O3" t="s">
-        <v>179</v>
-      </c>
-      <c r="P3" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="R3" t="s">
-        <v>245</v>
-      </c>
-      <c r="S3" t="s">
-        <v>173</v>
-      </c>
-      <c r="T3" t="s">
-        <v>245</v>
-      </c>
-      <c r="U3" t="s">
-        <v>238</v>
+      <c r="K12" t="s">
+        <v>313</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="M12" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N12" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="O12" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="P12" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q12" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S12" t="s">
+        <v>238</v>
+      </c>
+      <c r="T12" t="s">
+        <v>173</v>
+      </c>
+      <c r="U12" t="s">
+        <v>238</v>
+      </c>
+      <c r="V12" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A13" s="8">
+        <v>30675939</v>
+      </c>
+      <c r="B13" t="s">
+        <v>238</v>
+      </c>
+      <c r="C13" t="s">
+        <v>238</v>
+      </c>
+      <c r="D13" t="s">
+        <v>367</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="G13" t="s">
+        <v>173</v>
+      </c>
+      <c r="H13" t="s">
+        <v>238</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="J13" t="s">
+        <v>175</v>
+      </c>
+      <c r="K13" t="s">
+        <v>313</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="M13" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N13" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="O13" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="P13" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q13" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S13" t="s">
+        <v>238</v>
+      </c>
+      <c r="T13" t="s">
+        <v>173</v>
+      </c>
+      <c r="U13" t="s">
+        <v>238</v>
+      </c>
+      <c r="V13" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="B14" t="s">
+        <v>238</v>
+      </c>
+      <c r="C14" t="s">
+        <v>238</v>
+      </c>
+      <c r="D14" t="s">
+        <v>367</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="G14" t="s">
+        <v>173</v>
+      </c>
+      <c r="H14" t="s">
+        <v>238</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="J14" t="s">
+        <v>175</v>
+      </c>
+      <c r="K14" t="s">
+        <v>313</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="M14" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N14" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="O14" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="P14" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q14" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S14" t="s">
+        <v>238</v>
+      </c>
+      <c r="T14" t="s">
+        <v>173</v>
+      </c>
+      <c r="U14" t="s">
+        <v>238</v>
+      </c>
+      <c r="V14" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15" s="8">
+        <v>30680193</v>
+      </c>
+      <c r="B15" t="s">
+        <v>238</v>
+      </c>
+      <c r="C15" t="s">
+        <v>238</v>
+      </c>
+      <c r="D15" t="s">
+        <v>367</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="G15" t="s">
+        <v>173</v>
+      </c>
+      <c r="H15" t="s">
+        <v>238</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="J15" t="s">
+        <v>175</v>
+      </c>
+      <c r="K15" t="s">
+        <v>313</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="M15" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N15" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="O15" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="P15" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q15" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S15" t="s">
+        <v>238</v>
+      </c>
+      <c r="T15" t="s">
+        <v>173</v>
+      </c>
+      <c r="U15" t="s">
+        <v>238</v>
+      </c>
+      <c r="V15" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A16" s="8">
+        <v>33625608</v>
+      </c>
+      <c r="B16" t="s">
+        <v>238</v>
+      </c>
+      <c r="C16" t="s">
+        <v>238</v>
+      </c>
+      <c r="D16" t="s">
+        <v>367</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="G16" t="s">
+        <v>173</v>
+      </c>
+      <c r="H16" t="s">
+        <v>238</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="J16" t="s">
+        <v>175</v>
+      </c>
+      <c r="K16" t="s">
+        <v>313</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="M16" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N16" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="O16" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="P16" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q16" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S16" t="s">
+        <v>238</v>
+      </c>
+      <c r="T16" t="s">
+        <v>173</v>
+      </c>
+      <c r="U16" t="s">
+        <v>238</v>
+      </c>
+      <c r="V16" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A17" s="8">
+        <v>30675154</v>
+      </c>
+      <c r="B17" t="s">
+        <v>238</v>
+      </c>
+      <c r="C17" t="s">
+        <v>238</v>
+      </c>
+      <c r="D17" t="s">
+        <v>367</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="G17" t="s">
+        <v>173</v>
+      </c>
+      <c r="H17" t="s">
+        <v>238</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="J17" t="s">
+        <v>175</v>
+      </c>
+      <c r="K17" t="s">
+        <v>313</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="M17" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N17" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="O17" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="P17" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q17" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S17" t="s">
+        <v>238</v>
+      </c>
+      <c r="T17" t="s">
+        <v>173</v>
+      </c>
+      <c r="U17" t="s">
+        <v>238</v>
+      </c>
+      <c r="V17" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A18" s="21" t="s">
+        <v>372</v>
+      </c>
+      <c r="B18" t="s">
+        <v>238</v>
+      </c>
+      <c r="C18" t="s">
+        <v>238</v>
+      </c>
+      <c r="D18" t="s">
+        <v>367</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="G18" t="s">
+        <v>173</v>
+      </c>
+      <c r="H18" t="s">
+        <v>238</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="J18" t="s">
+        <v>175</v>
+      </c>
+      <c r="K18" t="s">
+        <v>313</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="M18" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N18" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="O18" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="P18" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q18" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S18" t="s">
+        <v>238</v>
+      </c>
+      <c r="T18" t="s">
+        <v>173</v>
+      </c>
+      <c r="U18" t="s">
+        <v>238</v>
+      </c>
+      <c r="V18" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{58F1D4E0-6B9B-C441-8606-201BFF7DA851}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{E098BFA3-6597-C946-B98F-048C45A101AC}"/>
+    <hyperlink ref="E6" r:id="rId1" xr:uid="{F63FA05B-C9C0-C04F-A338-C2F3625D34B0}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{4E430D97-9DD1-E246-AB78-3E8C822FAA53}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{B4760093-B93C-8343-AD78-C6348CA39DEF}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{16BCE04F-949F-C44C-A8DA-1A21D82F73CC}"/>
+    <hyperlink ref="M12:M18" r:id="rId5" display="Seg@123" xr:uid="{8474FF47-7614-9644-9C4F-8A9A41D1D9E3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC304399-42DC-F242-AC29-559004AE5CDE}">
+  <dimension ref="A1:V20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:V18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="29" customWidth="1"/>
+    <col min="9" max="9" width="24.5" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H1" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J1" t="s">
+        <v>165</v>
+      </c>
+      <c r="K1" t="s">
+        <v>144</v>
+      </c>
+      <c r="L1" t="s">
+        <v>166</v>
+      </c>
+      <c r="M1" t="s">
+        <v>167</v>
+      </c>
+      <c r="N1" t="s">
+        <v>168</v>
+      </c>
+      <c r="O1" t="s">
+        <v>169</v>
+      </c>
+      <c r="P1" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>171</v>
+      </c>
+      <c r="R1" t="s">
+        <v>233</v>
+      </c>
+      <c r="S1" t="s">
+        <v>234</v>
+      </c>
+      <c r="T1" t="s">
+        <v>235</v>
+      </c>
+      <c r="U1" t="s">
+        <v>236</v>
+      </c>
+      <c r="V1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" s="10">
+        <v>30672647</v>
+      </c>
+      <c r="B2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D2" t="s">
+        <v>367</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="G2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H2" t="s">
+        <v>238</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="J2" t="s">
+        <v>175</v>
+      </c>
+      <c r="K2" t="s">
+        <v>313</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="M2" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N2" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="O2" s="20" t="s">
+        <v>370</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S2" t="s">
+        <v>238</v>
+      </c>
+      <c r="T2" t="s">
+        <v>173</v>
+      </c>
+      <c r="U2" t="s">
+        <v>238</v>
+      </c>
+      <c r="V2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" s="10">
+        <v>30681138</v>
+      </c>
+      <c r="B3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C3" t="s">
+        <v>238</v>
+      </c>
+      <c r="D3" t="s">
+        <v>367</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="G3" t="s">
+        <v>173</v>
+      </c>
+      <c r="H3" t="s">
+        <v>238</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="J3" t="s">
+        <v>175</v>
+      </c>
+      <c r="K3" t="s">
+        <v>313</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>354</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N3" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="O3" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="P3" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q3" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S3" t="s">
+        <v>238</v>
+      </c>
+      <c r="T3" t="s">
+        <v>173</v>
+      </c>
+      <c r="U3" t="s">
+        <v>238</v>
+      </c>
+      <c r="V3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" s="10">
+        <v>30674440</v>
+      </c>
+      <c r="B4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D4" t="s">
+        <v>367</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="F4" s="17">
+        <v>30672647</v>
+      </c>
+      <c r="G4" t="s">
+        <v>173</v>
+      </c>
+      <c r="H4" t="s">
+        <v>238</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>360</v>
+      </c>
+      <c r="J4" t="s">
+        <v>175</v>
+      </c>
+      <c r="K4" t="s">
+        <v>313</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="M4" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N4" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="O4" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="P4" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q4" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S4" t="s">
+        <v>238</v>
+      </c>
+      <c r="T4" t="s">
+        <v>173</v>
+      </c>
+      <c r="U4" t="s">
+        <v>238</v>
+      </c>
+      <c r="V4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5" s="10">
+        <v>30681496</v>
+      </c>
+      <c r="B5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D5" t="s">
+        <v>367</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="G5" t="s">
+        <v>173</v>
+      </c>
+      <c r="H5" t="s">
+        <v>238</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>362</v>
+      </c>
+      <c r="J5" t="s">
+        <v>175</v>
+      </c>
+      <c r="K5" t="s">
+        <v>313</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="M5" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N5" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="O5" s="20" t="s">
+        <v>370</v>
+      </c>
+      <c r="P5" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q5" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S5" t="s">
+        <v>238</v>
+      </c>
+      <c r="T5" t="s">
+        <v>173</v>
+      </c>
+      <c r="U5" t="s">
+        <v>238</v>
+      </c>
+      <c r="V5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="10">
+        <v>30678703</v>
+      </c>
+      <c r="B6" t="s">
+        <v>238</v>
+      </c>
+      <c r="C6" t="s">
+        <v>238</v>
+      </c>
+      <c r="D6" t="s">
+        <v>367</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>364</v>
+      </c>
+      <c r="G6" t="s">
+        <v>173</v>
+      </c>
+      <c r="H6" t="s">
+        <v>238</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="J6" t="s">
+        <v>175</v>
+      </c>
+      <c r="K6" t="s">
+        <v>313</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="M6" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N6" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="O6" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="P6" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q6" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S6" t="s">
+        <v>238</v>
+      </c>
+      <c r="T6" t="s">
+        <v>173</v>
+      </c>
+      <c r="U6" t="s">
+        <v>238</v>
+      </c>
+      <c r="V6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>32087330</v>
+      </c>
+      <c r="B7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C7" t="s">
+        <v>238</v>
+      </c>
+      <c r="D7" t="s">
+        <v>367</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="G7" t="s">
+        <v>173</v>
+      </c>
+      <c r="H7" t="s">
+        <v>238</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="J7" t="s">
+        <v>175</v>
+      </c>
+      <c r="K7" t="s">
+        <v>313</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="M7" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N7" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="O7" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="P7" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q7" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S7" t="s">
+        <v>238</v>
+      </c>
+      <c r="T7" t="s">
+        <v>173</v>
+      </c>
+      <c r="U7" t="s">
+        <v>238</v>
+      </c>
+      <c r="V7" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>31175834</v>
+      </c>
+      <c r="B8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C8" t="s">
+        <v>238</v>
+      </c>
+      <c r="D8" t="s">
+        <v>367</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="G8" t="s">
+        <v>173</v>
+      </c>
+      <c r="H8" t="s">
+        <v>238</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="J8" t="s">
+        <v>175</v>
+      </c>
+      <c r="K8" t="s">
+        <v>313</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N8" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="O8" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="P8" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q8" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S8" t="s">
+        <v>238</v>
+      </c>
+      <c r="T8" t="s">
+        <v>173</v>
+      </c>
+      <c r="U8" t="s">
+        <v>238</v>
+      </c>
+      <c r="V8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>33625544</v>
+      </c>
+      <c r="B9" t="s">
+        <v>238</v>
+      </c>
+      <c r="C9" t="s">
+        <v>238</v>
+      </c>
+      <c r="D9" t="s">
+        <v>367</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="G9" t="s">
+        <v>173</v>
+      </c>
+      <c r="H9" t="s">
+        <v>238</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="J9" t="s">
+        <v>175</v>
+      </c>
+      <c r="K9" t="s">
+        <v>313</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="M9" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N9" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="O9" s="20" t="s">
+        <v>370</v>
+      </c>
+      <c r="P9" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q9" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S9" t="s">
+        <v>238</v>
+      </c>
+      <c r="T9" t="s">
+        <v>173</v>
+      </c>
+      <c r="U9" t="s">
+        <v>238</v>
+      </c>
+      <c r="V9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
+        <v>30682333</v>
+      </c>
+      <c r="B10" t="s">
+        <v>238</v>
+      </c>
+      <c r="C10" t="s">
+        <v>238</v>
+      </c>
+      <c r="D10" t="s">
+        <v>367</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="G10" t="s">
+        <v>173</v>
+      </c>
+      <c r="H10" t="s">
+        <v>238</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="J10" t="s">
+        <v>175</v>
+      </c>
+      <c r="K10" t="s">
+        <v>313</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="M10" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N10" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="O10" s="20" t="s">
+        <v>370</v>
+      </c>
+      <c r="P10" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q10" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S10" t="s">
+        <v>238</v>
+      </c>
+      <c r="T10" t="s">
+        <v>173</v>
+      </c>
+      <c r="U10" t="s">
+        <v>238</v>
+      </c>
+      <c r="V10" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A11" s="8">
+        <v>33625753</v>
+      </c>
+      <c r="B11" t="s">
+        <v>238</v>
+      </c>
+      <c r="C11" t="s">
+        <v>238</v>
+      </c>
+      <c r="D11" t="s">
+        <v>367</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="G11" t="s">
+        <v>173</v>
+      </c>
+      <c r="H11" t="s">
+        <v>238</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="J11" t="s">
+        <v>175</v>
+      </c>
+      <c r="K11" t="s">
+        <v>313</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="M11" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N11" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="O11" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="P11" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q11" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S11" t="s">
+        <v>238</v>
+      </c>
+      <c r="T11" t="s">
+        <v>173</v>
+      </c>
+      <c r="U11" t="s">
+        <v>238</v>
+      </c>
+      <c r="V11" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A12" s="8">
+        <v>31621727</v>
+      </c>
+      <c r="B12" t="s">
+        <v>238</v>
+      </c>
+      <c r="C12" t="s">
+        <v>238</v>
+      </c>
+      <c r="D12" t="s">
+        <v>367</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="G12" t="s">
+        <v>173</v>
+      </c>
+      <c r="H12" t="s">
+        <v>238</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="J12" t="s">
+        <v>175</v>
+      </c>
+      <c r="K12" t="s">
+        <v>313</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="M12" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N12" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="O12" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="P12" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q12" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S12" t="s">
+        <v>238</v>
+      </c>
+      <c r="T12" t="s">
+        <v>173</v>
+      </c>
+      <c r="U12" t="s">
+        <v>238</v>
+      </c>
+      <c r="V12" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A13" s="8">
+        <v>30675939</v>
+      </c>
+      <c r="B13" t="s">
+        <v>238</v>
+      </c>
+      <c r="C13" t="s">
+        <v>238</v>
+      </c>
+      <c r="D13" t="s">
+        <v>367</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="G13" t="s">
+        <v>173</v>
+      </c>
+      <c r="H13" t="s">
+        <v>238</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="J13" t="s">
+        <v>175</v>
+      </c>
+      <c r="K13" t="s">
+        <v>313</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="M13" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N13" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="O13" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="P13" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q13" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S13" t="s">
+        <v>238</v>
+      </c>
+      <c r="T13" t="s">
+        <v>173</v>
+      </c>
+      <c r="U13" t="s">
+        <v>238</v>
+      </c>
+      <c r="V13" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="B14" t="s">
+        <v>238</v>
+      </c>
+      <c r="C14" t="s">
+        <v>238</v>
+      </c>
+      <c r="D14" t="s">
+        <v>367</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="G14" t="s">
+        <v>173</v>
+      </c>
+      <c r="H14" t="s">
+        <v>238</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="J14" t="s">
+        <v>175</v>
+      </c>
+      <c r="K14" t="s">
+        <v>313</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="M14" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N14" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="O14" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="P14" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q14" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S14" t="s">
+        <v>238</v>
+      </c>
+      <c r="T14" t="s">
+        <v>173</v>
+      </c>
+      <c r="U14" t="s">
+        <v>238</v>
+      </c>
+      <c r="V14" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15" s="8">
+        <v>30680193</v>
+      </c>
+      <c r="B15" t="s">
+        <v>238</v>
+      </c>
+      <c r="C15" t="s">
+        <v>238</v>
+      </c>
+      <c r="D15" t="s">
+        <v>367</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="G15" t="s">
+        <v>173</v>
+      </c>
+      <c r="H15" t="s">
+        <v>238</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="J15" t="s">
+        <v>175</v>
+      </c>
+      <c r="K15" t="s">
+        <v>313</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="M15" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N15" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="O15" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="P15" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q15" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S15" t="s">
+        <v>238</v>
+      </c>
+      <c r="T15" t="s">
+        <v>173</v>
+      </c>
+      <c r="U15" t="s">
+        <v>238</v>
+      </c>
+      <c r="V15" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A16" s="8">
+        <v>33625608</v>
+      </c>
+      <c r="B16" t="s">
+        <v>238</v>
+      </c>
+      <c r="C16" t="s">
+        <v>238</v>
+      </c>
+      <c r="D16" t="s">
+        <v>367</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="G16" t="s">
+        <v>173</v>
+      </c>
+      <c r="H16" t="s">
+        <v>238</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="J16" t="s">
+        <v>175</v>
+      </c>
+      <c r="K16" t="s">
+        <v>313</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="M16" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N16" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="O16" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="P16" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q16" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S16" t="s">
+        <v>238</v>
+      </c>
+      <c r="T16" t="s">
+        <v>173</v>
+      </c>
+      <c r="U16" t="s">
+        <v>238</v>
+      </c>
+      <c r="V16" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A17" s="8">
+        <v>30675154</v>
+      </c>
+      <c r="B17" t="s">
+        <v>238</v>
+      </c>
+      <c r="C17" t="s">
+        <v>238</v>
+      </c>
+      <c r="D17" t="s">
+        <v>367</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="G17" t="s">
+        <v>173</v>
+      </c>
+      <c r="H17" t="s">
+        <v>238</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="J17" t="s">
+        <v>175</v>
+      </c>
+      <c r="K17" t="s">
+        <v>313</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="M17" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N17" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="O17" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="P17" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q17" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S17" t="s">
+        <v>238</v>
+      </c>
+      <c r="T17" t="s">
+        <v>173</v>
+      </c>
+      <c r="U17" t="s">
+        <v>238</v>
+      </c>
+      <c r="V17" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="B18" t="s">
+        <v>238</v>
+      </c>
+      <c r="C18" t="s">
+        <v>238</v>
+      </c>
+      <c r="D18" t="s">
+        <v>367</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="G18" t="s">
+        <v>173</v>
+      </c>
+      <c r="H18" t="s">
+        <v>238</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="J18" t="s">
+        <v>175</v>
+      </c>
+      <c r="K18" t="s">
+        <v>313</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="M18" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="N18" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="O18" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="P18" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q18" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="S18" t="s">
+        <v>238</v>
+      </c>
+      <c r="T18" t="s">
+        <v>173</v>
+      </c>
+      <c r="U18" t="s">
+        <v>238</v>
+      </c>
+      <c r="V18" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A20" s="10"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="17"/>
+      <c r="I20" s="15"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E6" r:id="rId1" xr:uid="{EBDF1D69-D51A-9C42-9C9A-DEE2258B84F8}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{A098325D-4A6D-DE4D-B277-50BFB213FD40}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{5F72EF14-6881-B349-B735-E742308A880A}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{775028D0-3190-B54E-B3DB-0A246AFC5E20}"/>
+    <hyperlink ref="M12:M23" r:id="rId5" display="Seg@123" xr:uid="{2D4D9FCC-EABE-1E4F-A84F-4809C66511CB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0588CAB-E2D0-C44A-A810-90E391CD495F}">
   <dimension ref="A1:R3"/>
   <sheetViews>
@@ -2394,210 +4963,170 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F1" t="s">
         <v>181</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
         <v>182</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>183</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>184</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>185</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>186</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>187</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
         <v>188</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>189</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
         <v>190</v>
       </c>
-      <c r="K1" t="s">
+      <c r="P1" t="s">
         <v>191</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q1" t="s">
         <v>192</v>
       </c>
-      <c r="M1" t="s">
+      <c r="R1" t="s">
         <v>193</v>
-      </c>
-      <c r="N1" t="s">
-        <v>194</v>
-      </c>
-      <c r="O1" t="s">
-        <v>195</v>
-      </c>
-      <c r="P1" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>197</v>
-      </c>
-      <c r="R1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="B2" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="C2" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="G2" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="H2" t="s">
+        <v>283</v>
+      </c>
+      <c r="I2" t="s">
+        <v>197</v>
+      </c>
+      <c r="J2" t="s">
+        <v>272</v>
+      </c>
+      <c r="K2" t="s">
         <v>298</v>
-      </c>
-      <c r="I2" t="s">
-        <v>202</v>
-      </c>
-      <c r="J2" t="s">
-        <v>286</v>
-      </c>
-      <c r="K2" t="s">
-        <v>315</v>
       </c>
       <c r="L2" t="s">
         <v>128</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="P2" t="s">
         <v>128</v>
       </c>
       <c r="Q2" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="R2" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="B3" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="C3" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="G3" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="I3" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="J3" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="K3" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="L3" t="s">
         <v>128</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="P3" t="s">
         <v>128</v>
       </c>
       <c r="Q3" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="R3" t="s">
-        <v>280</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E7C2F2-6F0A-B443-B65C-575B7D4BE1AE}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" customWidth="true" width="14.83203125" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>299</v>
-      </c>
-      <c r="C1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>52</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -2606,66 +5135,47 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D54A9207-92E4-9C42-B04A-2202B7F6AC1F}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E7C2F2-6F0A-B443-B65C-575B7D4BE1AE}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="30.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="14.83203125" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B1" t="s">
-        <v>302</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>303</v>
+        <v>284</v>
       </c>
       <c r="D1" t="s">
-        <v>304</v>
-      </c>
-      <c r="E1" t="s">
-        <v>305</v>
-      </c>
-      <c r="F1" t="s">
-        <v>306</v>
-      </c>
-      <c r="G1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>307</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="C2" t="s">
-        <v>309</v>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>313</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="E2" t="s">
-        <v>311</v>
-      </c>
-      <c r="F2" t="s">
-        <v>312</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>313</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{A874FBE6-5016-5249-8162-86EB24D7EEB0}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{AA32AAB6-0053-7D4D-842C-26AC3E9349D0}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2680,7 +5190,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="2" max="2" width="33" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -3031,6 +5541,70 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D54A9207-92E4-9C42-B04A-2202B7F6AC1F}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="30.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E1" t="s">
+        <v>289</v>
+      </c>
+      <c r="F1" t="s">
+        <v>290</v>
+      </c>
+      <c r="G1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="E2" t="s">
+        <v>295</v>
+      </c>
+      <c r="F2" t="s">
+        <v>296</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>297</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{AA32AAB6-0053-7D4D-842C-26AC3E9349D0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B93804DE-5A82-C043-BB14-CD95D1BBB58D}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -3040,26 +5614,26 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="17.1640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.5" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="B1" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="C1" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="D1" t="s">
         <v>144</v>
       </c>
       <c r="E1" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -3070,13 +5644,13 @@
         <v>174</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="D2" t="s">
         <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -3097,9 +5671,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="23.83203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.5" collapsed="true"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.83203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -3462,161 +6036,161 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="35.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="20.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="23.5" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="25.1640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="19.5" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="25.33203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="25.6640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="32.5" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="40.1640625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="28.1640625" collapsed="true"/>
+    <col min="1" max="1" width="35" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="25.1640625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="31" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="25.33203125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25.6640625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.5" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="25" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="40.1640625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="27" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="28.1640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H1" t="s">
         <v>207</v>
       </c>
-      <c r="C1" t="s">
+      <c r="I1" t="s">
         <v>208</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J1" t="s">
         <v>209</v>
       </c>
-      <c r="E1" t="s">
+      <c r="K1" t="s">
         <v>210</v>
       </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M1" t="s">
         <v>211</v>
       </c>
-      <c r="G1" t="s">
+      <c r="N1" t="s">
         <v>212</v>
       </c>
-      <c r="H1" t="s">
-        <v>213</v>
-      </c>
-      <c r="I1" t="s">
-        <v>214</v>
-      </c>
-      <c r="J1" t="s">
-        <v>215</v>
-      </c>
-      <c r="K1" t="s">
-        <v>216</v>
-      </c>
-      <c r="L1" t="s">
-        <v>219</v>
-      </c>
-      <c r="M1" t="s">
-        <v>217</v>
-      </c>
-      <c r="N1" t="s">
-        <v>218</v>
-      </c>
       <c r="O1" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B2" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="D2" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>52</v>
       </c>
       <c r="G2" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="H2" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="J2" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="K2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="L2" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="N2" t="s">
+        <v>219</v>
+      </c>
+      <c r="O2" t="s">
         <v>231</v>
-      </c>
-      <c r="N2" t="s">
-        <v>225</v>
-      </c>
-      <c r="O2" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C3" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="D3" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E3" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>53</v>
       </c>
       <c r="G3" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="H3" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="J3" t="s">
+        <v>276</v>
+      </c>
+      <c r="K3" t="s">
+        <v>230</v>
+      </c>
+      <c r="L3" t="s">
+        <v>224</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="N3" t="s">
+        <v>229</v>
+      </c>
+      <c r="O3" t="s">
         <v>231</v>
-      </c>
-      <c r="J3" t="s">
-        <v>291</v>
-      </c>
-      <c r="K3" t="s">
-        <v>236</v>
-      </c>
-      <c r="L3" t="s">
-        <v>230</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="N3" t="s">
-        <v>235</v>
-      </c>
-      <c r="O3" t="s">
-        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -3634,11 +6208,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.83203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="20.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.1640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.83203125" collapsed="true"/>
+    <col min="1" max="1" width="14.83203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -3666,10 +6240,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="B2" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="C2" t="s">
         <v>126</v>
@@ -3678,90 +6252,90 @@
         <v>142</v>
       </c>
       <c r="E2" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="B3" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="C3" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>142</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="B4" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="C4" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>142</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="B5" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="C5" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>142</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B6" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C6" t="s">
         <v>126</v>
@@ -3770,13 +6344,13 @@
         <v>127</v>
       </c>
       <c r="E6" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -3812,7 +6386,7 @@
         <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="G1" t="s">
         <v>136</v>
@@ -3833,7 +6407,7 @@
         <v>141</v>
       </c>
       <c r="M1" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -3853,13 +6427,13 @@
         <v>128</v>
       </c>
       <c r="F2" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>142</v>
       </c>
       <c r="H2" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>142</v>
@@ -3874,7 +6448,7 @@
         <v>143</v>
       </c>
       <c r="M2" t="s">
-        <v>261</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -3885,40 +6459,49 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CE29F11-D419-E34D-8103-7F124FCAB900}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.33203125" collapsed="true"/>
+    <col min="3" max="3" width="21" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>262</v>
-      </c>
-      <c r="B2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>263</v>
-      </c>
-      <c r="B3" t="s">
-        <v>128</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -3929,39 +6512,70 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E414F2-882A-9B4E-99BF-1CD7EF37A74D}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" width="16.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>246</v>
-      </c>
-      <c r="B2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>264</v>
-      </c>
-      <c r="B3" t="s">
-        <v>128</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>